<commit_message>
couple more tdreader tests
</commit_message>
<xml_diff>
--- a/Test/test_td_hits_file.xlsx
+++ b/Test/test_td_hits_file.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="43">
   <si>
     <t>PFR</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>RESID:929292@94</t>
+  </si>
+  <si>
+    <t>XTESALSYAALILADSEIEISSEKLLTLTNAANVPVENIWADIFAKALDGQNLKDLLVNFSAGAAAPAGVAGGVAGGEAGEAEAEKEEEEAKEESDDDMGFGLFD</t>
   </si>
 </sst>
 </file>
@@ -523,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X6"/>
+  <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:U1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,76 +755,76 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>11032</v>
+        <v>71601</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="H4">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="I4" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="J4" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="K4" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="L4" t="s">
         <v>24</v>
       </c>
       <c r="M4">
-        <v>8298.4705146899996</v>
+        <v>10892.19524069</v>
       </c>
       <c r="N4">
-        <v>8303.8127800000002</v>
+        <v>10898.767680000001</v>
       </c>
       <c r="O4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="P4" t="s">
         <v>25</v>
       </c>
       <c r="Q4">
-        <v>8298.4723288448895</v>
+        <v>10892.207744777499</v>
       </c>
       <c r="R4">
-        <v>1034</v>
+        <v>848</v>
       </c>
       <c r="S4">
-        <v>91.885243333333307</v>
+        <v>75.501321666666698</v>
       </c>
       <c r="T4">
-        <v>4.5889431901253599E-114</v>
+        <v>1.08534775914209E-126</v>
       </c>
       <c r="U4">
-        <v>2.2659899102903199E-76</v>
+        <v>1.3356636290276699E-84</v>
       </c>
       <c r="V4">
-        <v>1.18862953942261E-70</v>
+        <v>7.0057427271582204E-79</v>
       </c>
       <c r="W4">
-        <v>860.62255867077602</v>
+        <v>494.23473928831999</v>
       </c>
       <c r="X4">
-        <v>0.4</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -868,34 +871,34 @@
         <v>8303.8127800000002</v>
       </c>
       <c r="O5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P5" t="s">
         <v>25</v>
       </c>
       <c r="Q5">
-        <v>8298.4758992368097</v>
+        <v>8298.4723288448895</v>
       </c>
       <c r="R5">
-        <v>1023</v>
+        <v>1034</v>
       </c>
       <c r="S5">
-        <v>92.001024999999998</v>
+        <v>91.885243333333307</v>
       </c>
       <c r="T5">
-        <v>1.04102283390667E-107</v>
+        <v>4.5889431901253599E-114</v>
       </c>
       <c r="U5">
-        <v>3.2638036277088602E-72</v>
+        <v>2.2659899102903199E-76</v>
       </c>
       <c r="V5">
-        <v>1.71194986162762E-66</v>
+        <v>1.18862953942261E-70</v>
       </c>
       <c r="W5">
-        <v>1066.8577483884701</v>
+        <v>860.62255867077602</v>
       </c>
       <c r="X5">
-        <v>0.33333333333333298</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -942,33 +945,107 @@
         <v>8303.8127800000002</v>
       </c>
       <c r="O6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P6" t="s">
         <v>25</v>
       </c>
       <c r="Q6">
+        <v>8298.4758992368097</v>
+      </c>
+      <c r="R6">
+        <v>1023</v>
+      </c>
+      <c r="S6">
+        <v>92.001024999999998</v>
+      </c>
+      <c r="T6">
+        <v>1.04102283390667E-107</v>
+      </c>
+      <c r="U6">
+        <v>3.2638036277088602E-72</v>
+      </c>
+      <c r="V6">
+        <v>1.71194986162762E-66</v>
+      </c>
+      <c r="W6">
+        <v>1066.8577483884701</v>
+      </c>
+      <c r="X6">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>11032</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>77</v>
+      </c>
+      <c r="H7">
+        <v>76</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7">
+        <v>8298.4705146899996</v>
+      </c>
+      <c r="N7">
+        <v>8303.8127800000002</v>
+      </c>
+      <c r="O7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q7">
         <v>8298.4770076489604</v>
       </c>
-      <c r="R6">
+      <c r="R7">
         <v>1286</v>
       </c>
-      <c r="S6">
+      <c r="S7">
         <v>116.20425</v>
       </c>
-      <c r="T6">
+      <c r="T7">
         <v>2.2024558973003701E-9</v>
       </c>
-      <c r="U6">
+      <c r="U7">
         <v>5.5880138875496503E-8</v>
       </c>
-      <c r="V6">
+      <c r="V7">
         <v>2.9312038607419402E-2</v>
       </c>
-      <c r="W6">
+      <c r="W7">
         <v>380.77767402934097</v>
       </c>
-      <c r="X6">
+      <c r="X7">
         <v>6.6666666666666693E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
calibration bug fixes and neucode td
</commit_message>
<xml_diff>
--- a/Test/test_td_hits_file.xlsx
+++ b/Test/test_td_hits_file.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -131,9 +131,6 @@
     <t>60S acidic ribosomal protein P1-alpha</t>
   </si>
   <si>
-    <t>STESALSYAALILADSEIEISSEKLLTLTNAANVPVENIWADIFAKALDGQNLKDLLVNFSAGAAAPAGVAGGVAGGEAGEAEAEKEEEEAKEESDDDMGFGLFD</t>
-  </si>
-  <si>
     <t>alpha-amino acetylated residue@N, O-phospho-L-serine@95</t>
   </si>
   <si>
@@ -150,6 +147,9 @@
   </si>
   <si>
     <t>RESID:929292@94</t>
+  </si>
+  <si>
+    <t>SCESALSYAALILADSEIEISSEKLLTLTNAANVPVENIWADIFAKALDGQNLKDLLVNFSAGAAAPAGVAGGVAGGEAGEAEAEKEEEEAKEESDDDMGFGLFD</t>
   </si>
 </sst>
 </file>
@@ -525,11 +525,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="194.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -619,7 +623,7 @@
         <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -631,10 +635,10 @@
         <v>105</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" t="s">
         <v>40</v>
-      </c>
-      <c r="J2" t="s">
-        <v>41</v>
       </c>
       <c r="L2" t="s">
         <v>24</v>
@@ -646,13 +650,13 @@
         <v>10898.767680000001</v>
       </c>
       <c r="O2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P2" t="s">
         <v>25</v>
       </c>
       <c r="Q2">
-        <v>10892.207744777499</v>
+        <v>10894.13</v>
       </c>
       <c r="R2">
         <v>848</v>
@@ -690,7 +694,7 @@
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -702,13 +706,13 @@
         <v>105</v>
       </c>
       <c r="I3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" t="s">
         <v>36</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>37</v>
-      </c>
-      <c r="K3" t="s">
-        <v>38</v>
       </c>
       <c r="L3" t="s">
         <v>24</v>
@@ -720,13 +724,13 @@
         <v>10898.767680000001</v>
       </c>
       <c r="O3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P3" t="s">
         <v>25</v>
       </c>
       <c r="Q3">
-        <v>10892.207744777499</v>
+        <v>10894.13</v>
       </c>
       <c r="R3">
         <v>848</v>
@@ -764,7 +768,7 @@
         <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -776,13 +780,13 @@
         <v>105</v>
       </c>
       <c r="I4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" t="s">
         <v>36</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>37</v>
-      </c>
-      <c r="K4" t="s">
-        <v>38</v>
       </c>
       <c r="L4" t="s">
         <v>24</v>
@@ -794,13 +798,13 @@
         <v>10898.767680000001</v>
       </c>
       <c r="O4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P4" t="s">
         <v>25</v>
       </c>
       <c r="Q4">
-        <v>10892.207744777499</v>
+        <v>10894.13</v>
       </c>
       <c r="R4">
         <v>848</v>

</xml_diff>